<commit_message>
IPS estimación de componentes y dimensiones
</commit_message>
<xml_diff>
--- a/03_ips_clean/05_ips_utop_distop_long.xlsx
+++ b/03_ips_clean/05_ips_utop_distop_long.xlsx
@@ -940,7 +940,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="n">
-        <v>1.15558321354578</v>
+        <v>1.15558321354577</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
@@ -1130,7 +1130,7 @@
         <v>0</v>
       </c>
       <c r="C56" t="n">
-        <v>-0.54627143911055</v>
+        <v>-0.546271439110546</v>
       </c>
     </row>
   </sheetData>

</xml_diff>